<commit_message>
edit databaseExcel (28-07-67 22:14)
</commit_message>
<xml_diff>
--- a/เอกสาร/ฐานข้อมูล/DataDictionary.xlsx
+++ b/เอกสาร/ฐานข้อมูล/DataDictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27922"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\วิชาโครงการ\Project_subject_univesity\เอกสาร\ฐานข้อมูล\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\วิชาโครงการ\เอกสาร\ฐานข้อมูล\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E0CEA9-1385-4E2C-928F-A5B5A99E8665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86AFCB3B-486C-4944-AAAD-2FA7E58FDDF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ฐานข้อมูล" sheetId="14" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="337">
   <si>
     <t>Constraints</t>
   </si>
@@ -690,9 +690,6 @@
     <t>room_User_ID</t>
   </si>
   <si>
-    <t>Material((วัสดุ))</t>
-  </si>
-  <si>
     <t>mate_ID</t>
   </si>
   <si>
@@ -738,9 +735,6 @@
     <t>รหัสสภานะตำแหน่ง</t>
   </si>
   <si>
-    <t>รหัสสภานะวัสดุ</t>
-  </si>
-  <si>
     <t>จำนวน</t>
   </si>
   <si>
@@ -762,18 +756,6 @@
     <t>po_ID</t>
   </si>
   <si>
-    <t>po_user_id</t>
-  </si>
-  <si>
-    <t>po_saler</t>
-  </si>
-  <si>
-    <t>po_address</t>
-  </si>
-  <si>
-    <t>po_salerPhone</t>
-  </si>
-  <si>
     <t>po_Date</t>
   </si>
   <si>
@@ -792,9 +774,6 @@
     <t>ผู้ขาย</t>
   </si>
   <si>
-    <t>ที่อยู่</t>
-  </si>
-  <si>
     <t>วันที่ออกใบสั่งซื้อ</t>
   </si>
   <si>
@@ -807,29 +786,260 @@
     <t>วันที่อนุมัติ</t>
   </si>
   <si>
-    <t>po_MaterialBuy_ID</t>
-  </si>
-  <si>
-    <t>po_Appuser_id</t>
-  </si>
-  <si>
     <t>รหัสรายการสั่งซื้อ</t>
   </si>
   <si>
     <t>รหัสผู้อนุมัติ</t>
   </si>
   <si>
-    <t>po_totalPrice</t>
-  </si>
-  <si>
     <t>ราคารวม</t>
+  </si>
+  <si>
+    <t>POList((รายการสั่งซื้อ))</t>
+  </si>
+  <si>
+    <t>poli_ID</t>
+  </si>
+  <si>
+    <t>po_User_id</t>
+  </si>
+  <si>
+    <t>po_Saler</t>
+  </si>
+  <si>
+    <t>po_SalerPhone</t>
+  </si>
+  <si>
+    <t>po_TotalPrice</t>
+  </si>
+  <si>
+    <t>poli_Description</t>
+  </si>
+  <si>
+    <t>poli_Brand</t>
+  </si>
+  <si>
+    <t>poli_Model</t>
+  </si>
+  <si>
+    <t>poli_SerialNumber</t>
+  </si>
+  <si>
+    <t>poii_Qty</t>
+  </si>
+  <si>
+    <t>mate_SerialNumber</t>
+  </si>
+  <si>
+    <t>poli_Unit</t>
+  </si>
+  <si>
+    <t>poli_Price</t>
+  </si>
+  <si>
+    <t>poli_PO_ID</t>
+  </si>
+  <si>
+    <t>po_Appuser_ID</t>
+  </si>
+  <si>
+    <t>ที่อยู่ผู้ขาย</t>
+  </si>
+  <si>
+    <t>po_AddressSaler</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>Fk อาจผิด</t>
+  </si>
+  <si>
+    <t>MaterialStock((คลังวัสดุ))</t>
+  </si>
+  <si>
+    <t>รหัสสถานะวัสดุ</t>
+  </si>
+  <si>
+    <t>รายละเอียด</t>
+  </si>
+  <si>
+    <t>ราคาต่อหน่วย</t>
+  </si>
+  <si>
+    <t>จำนวนที่สั่ง</t>
+  </si>
+  <si>
+    <t>Withdrawal((เบิก))</t>
+  </si>
+  <si>
+    <t>withdrawal_ID</t>
+  </si>
+  <si>
+    <t>withdrawal_User_ID</t>
+  </si>
+  <si>
+    <t>withdrawal_Mate_ID</t>
+  </si>
+  <si>
+    <t>withdrawal_Date</t>
+  </si>
+  <si>
+    <t>withdrawal_Status_ID</t>
+  </si>
+  <si>
+    <t>รหัสการเบิกวัสดุ</t>
+  </si>
+  <si>
+    <t>รหัสผู้เบิก</t>
+  </si>
+  <si>
+    <t>วันที่เบิก</t>
+  </si>
+  <si>
+    <t>withdrawal_Repair_ID</t>
+  </si>
+  <si>
+    <t>รหัสการแจ้งซ่อม</t>
+  </si>
+  <si>
+    <t>สถานะการเบิก</t>
+  </si>
+  <si>
+    <t>FOREIGN KEY (MaterialStock.mate_ID)</t>
+  </si>
+  <si>
+    <t>Repair((ซ่อม))</t>
+  </si>
+  <si>
+    <t>repair_ID</t>
+  </si>
+  <si>
+    <t>repair_User_ID</t>
+  </si>
+  <si>
+    <t>repair_Title</t>
+  </si>
+  <si>
+    <t>repair_Status_ID</t>
+  </si>
+  <si>
+    <t>ประเถทของการแก่ปัญหา</t>
+  </si>
+  <si>
+    <t>repair_RepairTyp_ID</t>
+  </si>
+  <si>
+    <t>repair_Description</t>
+  </si>
+  <si>
+    <t>RepairType((ประเภทการซ่อม))</t>
+  </si>
+  <si>
+    <t>stat_DateAdd</t>
+  </si>
+  <si>
+    <t>stat_dateEdit</t>
+  </si>
+  <si>
+    <t>รหัสผู้แจ้งซ่อม</t>
+  </si>
+  <si>
+    <t>หัวข้อ</t>
+  </si>
+  <si>
+    <t>รายละเอียดการแจ้งซ่อม</t>
+  </si>
+  <si>
+    <t>สถานะการแจ้งซ่อม</t>
+  </si>
+  <si>
+    <t>FOREIGN KEY (RepairType.repairTyp_ID</t>
+  </si>
+  <si>
+    <t>repairTyp_ID</t>
+  </si>
+  <si>
+    <t>repairTyp_Name</t>
+  </si>
+  <si>
+    <t>repairTyp_DateAdd</t>
+  </si>
+  <si>
+    <t>repairTyp_DateEdit</t>
+  </si>
+  <si>
+    <t>repairTyp_Status_ID</t>
+  </si>
+  <si>
+    <t>รหัสประเภทการซ่อม</t>
+  </si>
+  <si>
+    <t>ชื่อประเภทการซ่อม</t>
+  </si>
+  <si>
+    <t>RequestImages((รูปภาพ))</t>
+  </si>
+  <si>
+    <t>reqImg_Path</t>
+  </si>
+  <si>
+    <t>reqImg_ID</t>
+  </si>
+  <si>
+    <t>reqImg_Repair_ID</t>
+  </si>
+  <si>
+    <t>รหัสรูปภาพ</t>
+  </si>
+  <si>
+    <t>ที่อยู่รูปภาพ</t>
+  </si>
+  <si>
+    <t>FOREIGN KEY (Repair.repair_ID)</t>
+  </si>
+  <si>
+    <t>RepairTime((เวลาซ่อม))</t>
+  </si>
+  <si>
+    <t>repTime_ID</t>
+  </si>
+  <si>
+    <t>repTime_Repair_ID</t>
+  </si>
+  <si>
+    <t>repTime_StartTime</t>
+  </si>
+  <si>
+    <t>repTime_EndTime</t>
+  </si>
+  <si>
+    <t>repTime_User_ID</t>
+  </si>
+  <si>
+    <t>repTime_date</t>
+  </si>
+  <si>
+    <t>รหัสเวลาซ่อม</t>
+  </si>
+  <si>
+    <t>เวลาเริ่มซ่อม</t>
+  </si>
+  <si>
+    <t>เวลาสิ้นสุดการซ่อม</t>
+  </si>
+  <si>
+    <t>วันที่ซ่อม</t>
+  </si>
+  <si>
+    <t>รหัสช่างซ่อมบำรุง</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -840,6 +1050,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -883,15 +1100,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -901,9 +1115,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -922,9 +1140,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -962,9 +1180,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -997,26 +1215,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1049,26 +1250,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1251,23 +1435,23 @@
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>130</v>
       </c>
@@ -1281,7 +1465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1295,7 +1479,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1306,15 +1490,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>130</v>
       </c>
@@ -1328,7 +1512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1342,7 +1526,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1353,7 +1537,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1364,7 +1548,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1378,15 +1562,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>130</v>
       </c>
@@ -1400,7 +1584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1414,7 +1598,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1425,15 +1609,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>130</v>
       </c>
@@ -1447,7 +1631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -1461,7 +1645,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -1475,7 +1659,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -1486,7 +1670,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1497,7 +1681,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1508,7 +1692,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1519,7 +1703,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -1533,15 +1717,15 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>130</v>
       </c>
@@ -1555,7 +1739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -1569,7 +1753,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -1583,7 +1767,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>40</v>
       </c>
@@ -1594,7 +1778,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -1605,7 +1789,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -1616,7 +1800,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -1627,7 +1811,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>44</v>
       </c>
@@ -1638,15 +1822,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>130</v>
       </c>
@@ -1660,7 +1844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>47</v>
       </c>
@@ -1674,7 +1858,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>48</v>
       </c>
@@ -1688,7 +1872,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>49</v>
       </c>
@@ -1699,7 +1883,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>50</v>
       </c>
@@ -1710,7 +1894,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>51</v>
       </c>
@@ -1721,7 +1905,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -1732,7 +1916,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>53</v>
       </c>
@@ -1743,15 +1927,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="3" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>130</v>
       </c>
@@ -1765,7 +1949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>55</v>
       </c>
@@ -1779,7 +1963,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>56</v>
       </c>
@@ -1790,7 +1974,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>57</v>
       </c>
@@ -1801,7 +1985,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>58</v>
       </c>
@@ -1812,15 +1996,15 @@
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="3" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>130</v>
       </c>
@@ -1834,7 +2018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>63</v>
       </c>
@@ -1848,7 +2032,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>64</v>
       </c>
@@ -1862,7 +2046,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>65</v>
       </c>
@@ -1873,7 +2057,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>66</v>
       </c>
@@ -1884,7 +2068,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>67</v>
       </c>
@@ -1895,7 +2079,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>68</v>
       </c>
@@ -1906,7 +2090,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>69</v>
       </c>
@@ -1917,15 +2101,15 @@
         <v>78</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="3" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B57" s="6"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>130</v>
       </c>
@@ -1939,7 +2123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>80</v>
       </c>
@@ -1953,7 +2137,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>81</v>
       </c>
@@ -1967,7 +2151,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>82</v>
       </c>
@@ -1978,7 +2162,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>83</v>
       </c>
@@ -1989,15 +2173,15 @@
         <v>78</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" s="3" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="B63" s="3"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B63" s="6"/>
+      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>130</v>
       </c>
@@ -2011,7 +2195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>87</v>
       </c>
@@ -2025,7 +2209,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>88</v>
       </c>
@@ -2039,7 +2223,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>89</v>
       </c>
@@ -2050,7 +2234,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>90</v>
       </c>
@@ -2061,7 +2245,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>91</v>
       </c>
@@ -2072,7 +2256,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>92</v>
       </c>
@@ -2083,7 +2267,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>93</v>
       </c>
@@ -2094,15 +2278,15 @@
         <v>78</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="3" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="B72" s="3"/>
-      <c r="C72" s="3"/>
-      <c r="D72" s="3"/>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B72" s="6"/>
+      <c r="C72" s="6"/>
+      <c r="D72" s="6"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>130</v>
       </c>
@@ -2116,7 +2300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>101</v>
       </c>
@@ -2130,7 +2314,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>102</v>
       </c>
@@ -2144,7 +2328,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>103</v>
       </c>
@@ -2158,7 +2342,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>104</v>
       </c>
@@ -2169,7 +2353,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>105</v>
       </c>
@@ -2180,7 +2364,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>106</v>
       </c>
@@ -2191,15 +2375,15 @@
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" s="3" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="B80" s="3"/>
-      <c r="C80" s="3"/>
-      <c r="D80" s="3"/>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B80" s="6"/>
+      <c r="C80" s="6"/>
+      <c r="D80" s="6"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>130</v>
       </c>
@@ -2213,7 +2397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>112</v>
       </c>
@@ -2227,7 +2411,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>113</v>
       </c>
@@ -2241,7 +2425,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>114</v>
       </c>
@@ -2255,7 +2439,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>115</v>
       </c>
@@ -2266,7 +2450,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>116</v>
       </c>
@@ -2277,7 +2461,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>117</v>
       </c>
@@ -2288,15 +2472,15 @@
         <v>78</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A88" s="3" t="s">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="B88" s="3"/>
-      <c r="C88" s="3"/>
-      <c r="D88" s="3"/>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B88" s="6"/>
+      <c r="C88" s="6"/>
+      <c r="D88" s="6"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>130</v>
       </c>
@@ -2310,7 +2494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>122</v>
       </c>
@@ -2324,7 +2508,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>123</v>
       </c>
@@ -2338,7 +2522,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>124</v>
       </c>
@@ -2349,7 +2533,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>125</v>
       </c>
@@ -2360,7 +2544,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>126</v>
       </c>
@@ -2371,7 +2555,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>127</v>
       </c>
@@ -2382,7 +2566,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>128</v>
       </c>
@@ -2393,15 +2577,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A97" s="3" t="s">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="B97" s="3"/>
-      <c r="C97" s="3"/>
-      <c r="D97" s="3"/>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B97" s="6"/>
+      <c r="C97" s="6"/>
+      <c r="D97" s="6"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>130</v>
       </c>
@@ -2445,23 +2629,23 @@
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>130</v>
       </c>
@@ -2475,7 +2659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2489,7 +2673,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2500,7 +2684,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>147</v>
       </c>
@@ -2511,7 +2695,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -2525,15 +2709,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>130</v>
       </c>
@@ -2547,7 +2731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -2561,7 +2745,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -2572,7 +2756,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>150</v>
       </c>
@@ -2598,225 +2782,225 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C0966C1-10E6-4F48-BDCF-1F100D8FF618}">
-  <dimension ref="A1:E78"/>
+  <dimension ref="A1:E127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="D79" sqref="D79"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G93" sqref="G93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="44" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="5"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="4" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>130</v>
       </c>
@@ -2833,779 +3017,1457 @@
         <v>206</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="6"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="E19" s="6"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B22" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C22" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D22" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E22" s="5" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C24" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D24" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E24" s="3" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B25" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C25" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D25" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="5"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="5" t="s">
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B26" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C26" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="5" t="s">
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B27" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C27" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D27" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="E27" s="4" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B29" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C29" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D29" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E29" s="3" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="5" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B30" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C30" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D30" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E28" s="5"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="5" t="s">
+      <c r="E30" s="4"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B31" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C31" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D31" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="5"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="5" t="s">
+      <c r="E31" s="4"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B32" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C32" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D32" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="E30" s="5"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
+      <c r="E32" s="4"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="5" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B35" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C35" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D35" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E33" s="5"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="5" t="s">
+      <c r="E35" s="4"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B36" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C36" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="5" t="s">
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B37" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C37" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="5" t="s">
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="E42" s="4"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E43" s="4"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C49" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="B53" s="6"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="D66" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="E66" s="8" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="B67" t="s">
+        <v>278</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="B68" s="6"/>
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="6"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>243</v>
+      </c>
+      <c r="B70" t="s">
+        <v>248</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>259</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>260</v>
+      </c>
+      <c r="B72" t="s">
+        <v>249</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>274</v>
+      </c>
+      <c r="B73" t="s">
+        <v>273</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>261</v>
+      </c>
+      <c r="B74" t="s">
+        <v>161</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>244</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B75" t="s">
+        <v>250</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>245</v>
+      </c>
+      <c r="B76" t="s">
+        <v>251</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>247</v>
+      </c>
+      <c r="B77" t="s">
+        <v>252</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>246</v>
+      </c>
+      <c r="B78" t="s">
+        <v>253</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>272</v>
+      </c>
+      <c r="B79" t="s">
+        <v>255</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>262</v>
+      </c>
+      <c r="B80" t="s">
+        <v>256</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="B81" s="6"/>
+      <c r="C81" s="6"/>
+      <c r="D81" s="6"/>
+      <c r="E81" s="6"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>258</v>
+      </c>
+      <c r="B83" t="s">
+        <v>254</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>263</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>264</v>
+      </c>
+      <c r="B85" t="s">
+        <v>180</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>265</v>
+      </c>
+      <c r="B86" t="s">
+        <v>183</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>266</v>
+      </c>
+      <c r="B87" t="s">
         <v>184</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C87" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="B37" s="5" t="s">
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>267</v>
+      </c>
+      <c r="B88" t="s">
+        <v>281</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>269</v>
+      </c>
+      <c r="B89" t="s">
+        <v>62</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>270</v>
+      </c>
+      <c r="B90" t="s">
+        <v>280</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>271</v>
+      </c>
+      <c r="B91" t="s">
+        <v>118</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="B92" s="6"/>
+      <c r="C92" s="6"/>
+      <c r="D92" s="6"/>
+      <c r="E92" s="6"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>283</v>
+      </c>
+      <c r="B94" t="s">
+        <v>288</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D94" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>284</v>
+      </c>
+      <c r="B95" t="s">
+        <v>289</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="B96" t="s">
+        <v>59</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D96" s="4" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>286</v>
+      </c>
+      <c r="B97" t="s">
+        <v>290</v>
+      </c>
+      <c r="C97" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>291</v>
+      </c>
+      <c r="B98" t="s">
+        <v>292</v>
+      </c>
+      <c r="C98" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D98" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>287</v>
+      </c>
+      <c r="B99" t="s">
+        <v>293</v>
+      </c>
+      <c r="C99" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D99" s="4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="B100" s="6"/>
+      <c r="C100" s="6"/>
+      <c r="D100" s="6"/>
+      <c r="E100" s="6"/>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>296</v>
+      </c>
+      <c r="B102" t="s">
+        <v>292</v>
+      </c>
+      <c r="C102" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D102" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>297</v>
+      </c>
+      <c r="B103" t="s">
+        <v>306</v>
+      </c>
+      <c r="C103" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D103" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>298</v>
+      </c>
+      <c r="B104" t="s">
+        <v>307</v>
+      </c>
+      <c r="C104" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D104" s="4"/>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>301</v>
+      </c>
+      <c r="B105" t="s">
+        <v>300</v>
+      </c>
+      <c r="C105" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D105" s="4" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>302</v>
+      </c>
+      <c r="B106" t="s">
+        <v>308</v>
+      </c>
+      <c r="C106" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>299</v>
+      </c>
+      <c r="B107" t="s">
+        <v>309</v>
+      </c>
+      <c r="C107" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D107" s="4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="B108" s="6"/>
+      <c r="C108" s="6"/>
+      <c r="D108" s="6"/>
+      <c r="E108" s="6"/>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>311</v>
+      </c>
+      <c r="B110" t="s">
+        <v>316</v>
+      </c>
+      <c r="C110" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D110" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>312</v>
+      </c>
+      <c r="B111" t="s">
+        <v>317</v>
+      </c>
+      <c r="C111" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>313</v>
+      </c>
+      <c r="B112" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C112" t="s">
         <v>165</v>
       </c>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="B38" s="5" t="s">
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>314</v>
+      </c>
+      <c r="B113" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C113" t="s">
         <v>165</v>
       </c>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="C39" s="5" t="s">
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>315</v>
+      </c>
+      <c r="B114" t="s">
+        <v>74</v>
+      </c>
+      <c r="C114" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D114" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="E39" s="5" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="C40" s="5" t="s">
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="B115" s="6"/>
+      <c r="C115" s="6"/>
+      <c r="D115" s="6"/>
+      <c r="E115" s="6"/>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>320</v>
+      </c>
+      <c r="B117" t="s">
+        <v>322</v>
+      </c>
+      <c r="C117" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="D40" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="E40" s="5"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C41" s="5" t="s">
+      <c r="D117" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>319</v>
+      </c>
+      <c r="B118" t="s">
+        <v>323</v>
+      </c>
+      <c r="C118" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>321</v>
+      </c>
+      <c r="B119" t="s">
+        <v>292</v>
+      </c>
+      <c r="C119" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="D41" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="E41" s="5"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
+      <c r="D119" s="4" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="B120" s="6"/>
+      <c r="C120" s="6"/>
+      <c r="D120" s="6"/>
+      <c r="E120" s="6"/>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B121" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C121" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D121" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E121" s="1" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C44" s="5" t="s">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>326</v>
+      </c>
+      <c r="B122" t="s">
+        <v>332</v>
+      </c>
+      <c r="C122" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="D122" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="C46" s="5" t="s">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>328</v>
+      </c>
+      <c r="B123" t="s">
+        <v>333</v>
+      </c>
+      <c r="C123" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="C47" t="s">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>329</v>
+      </c>
+      <c r="B124" t="s">
+        <v>334</v>
+      </c>
+      <c r="C124" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="C49" s="5" t="s">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>331</v>
+      </c>
+      <c r="B125" t="s">
+        <v>335</v>
+      </c>
+      <c r="C125" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>327</v>
+      </c>
+      <c r="B126" t="s">
+        <v>292</v>
+      </c>
+      <c r="C126" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="D126" s="4" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>330</v>
+      </c>
+      <c r="B127" t="s">
+        <v>336</v>
+      </c>
+      <c r="C127" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D127" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A63" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="B63" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="C63" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="D63" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="E63" s="2"/>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A64" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="B64" t="s">
-        <v>238</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A65" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="B65" s="3"/>
-      <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
-      <c r="E65" s="3"/>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>245</v>
-      </c>
-      <c r="B67" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>246</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
-        <v>247</v>
-      </c>
-      <c r="B69" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
-        <v>248</v>
-      </c>
-      <c r="B70" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
-        <v>249</v>
-      </c>
-      <c r="B71" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>250</v>
-      </c>
-      <c r="B72" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>251</v>
-      </c>
-      <c r="B73" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>253</v>
-      </c>
-      <c r="B74" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>252</v>
-      </c>
-      <c r="B75" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A76" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
-        <v>262</v>
-      </c>
-      <c r="B77" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
-        <v>265</v>
-      </c>
-      <c r="B78" t="s">
-        <v>266</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A31:E31"/>
-    <mergeCell ref="A42:E42"/>
-    <mergeCell ref="A51:E51"/>
-    <mergeCell ref="A65:E65"/>
+  <mergeCells count="14">
+    <mergeCell ref="A100:E100"/>
+    <mergeCell ref="A108:E108"/>
+    <mergeCell ref="A115:E115"/>
+    <mergeCell ref="A120:E120"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A21:E21"/>
-    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="A92:E92"/>
+    <mergeCell ref="A81:E81"/>
+    <mergeCell ref="A33:E33"/>
+    <mergeCell ref="A44:E44"/>
+    <mergeCell ref="A53:E53"/>
+    <mergeCell ref="A68:E68"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>